<commit_message>
add flexible column selection in generic parser, #817
</commit_message>
<xml_diff>
--- a/bio_diversity/static/data_templates/measuring.xlsx
+++ b/bio_diversity/static/data_templates/measuring.xlsx
@@ -122,6 +122,19 @@
         </r>
       </text>
     </comment>
+    <comment ref="P3" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Enter extra columns pick in application here. All additional columns are Y/N variety.</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -295,7 +308,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
   <si>
     <t>PIT</t>
   </si>
@@ -358,6 +371,9 @@
   </si>
   <si>
     <t>UFID</t>
+  </si>
+  <si>
+    <t>ADDITIONAL COLUMNS</t>
   </si>
 </sst>
 </file>
@@ -491,7 +507,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -517,6 +533,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -806,10 +823,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:O71"/>
+  <dimension ref="A2:P71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -823,9 +840,10 @@
     <col min="11" max="11" width="14.140625" customWidth="1"/>
     <col min="13" max="13" width="14.140625" customWidth="1"/>
     <col min="15" max="15" width="12" customWidth="1"/>
+    <col min="16" max="16" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E2" s="10" t="s">
         <v>19</v>
       </c>
@@ -840,7 +858,7 @@
       <c r="N2" s="11"/>
       <c r="O2" s="12"/>
     </row>
-    <row r="3" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
@@ -886,75 +904,78 @@
       <c r="O3" s="9" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="P3" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C4" s="2"/>
       <c r="D4" s="4"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C5" s="2"/>
       <c r="D5" s="4"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
     </row>
-    <row r="6" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C6" s="2"/>
       <c r="D6" s="4"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C7" s="2"/>
       <c r="D7" s="1"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C8" s="2"/>
       <c r="D8" s="1"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C9" s="2"/>
       <c r="D9" s="1"/>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C10" s="2"/>
       <c r="D10" s="1"/>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C11" s="2"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C12" s="2"/>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C13" s="2"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C14" s="2"/>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C15" s="2"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C16" s="2"/>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>

</xml_diff>

<commit_message>
add mortatlity functionality to generic group parser
</commit_message>
<xml_diff>
--- a/bio_diversity/static/data_templates/measuring.xlsx
+++ b/bio_diversity/static/data_templates/measuring.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Individual" sheetId="3" r:id="rId1"/>
@@ -289,7 +289,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O3" authorId="0" shapeId="0">
+    <comment ref="P3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -308,7 +308,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="22">
   <si>
     <t>PIT</t>
   </si>
@@ -524,6 +524,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -533,7 +534,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -825,8 +825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:P71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1:L1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -844,19 +844,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
-      <c r="M2" s="11"/>
-      <c r="N2" s="11"/>
-      <c r="O2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="12"/>
+      <c r="O2" s="13"/>
     </row>
     <row r="3" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
@@ -904,7 +904,7 @@
       <c r="O3" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="P3" s="13" t="s">
+      <c r="P3" s="10" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1267,10 +1267,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:R71"/>
+  <dimension ref="A2:S71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3:I3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1:N1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1280,29 +1280,31 @@
     <col min="9" max="9" width="23.140625" customWidth="1"/>
     <col min="11" max="11" width="13" customWidth="1"/>
     <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="20.140625" customWidth="1"/>
-    <col min="16" max="16" width="16.28515625" customWidth="1"/>
-    <col min="17" max="17" width="22.140625" customWidth="1"/>
-    <col min="18" max="18" width="14" customWidth="1"/>
+    <col min="14" max="14" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="20.140625" customWidth="1"/>
+    <col min="17" max="17" width="16.28515625" customWidth="1"/>
+    <col min="18" max="18" width="22.140625" customWidth="1"/>
+    <col min="19" max="19" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D2" s="2"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
-      <c r="J2" s="10" t="s">
+      <c r="J2" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
-      <c r="M2" s="11"/>
-      <c r="N2" s="11"/>
-      <c r="O2" s="11"/>
-      <c r="P2" s="11"/>
-      <c r="Q2" s="11"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="12"/>
+      <c r="O2" s="12"/>
+      <c r="P2" s="12"/>
+      <c r="Q2" s="12"/>
       <c r="R2" s="12"/>
-    </row>
-    <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S2" s="13"/>
+    </row>
+    <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>17</v>
       </c>
@@ -1343,76 +1345,79 @@
         <v>4</v>
       </c>
       <c r="N3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="O3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="O3" s="5" t="s">
+      <c r="P3" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="P3" s="5" t="s">
+      <c r="Q3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="Q3" s="5" t="s">
+      <c r="R3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="R3" s="9" t="s">
+      <c r="S3" s="9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D4" s="2"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D5" s="2"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
     </row>
@@ -1638,7 +1643,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="J2:R2"/>
+    <mergeCell ref="J2:S2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add group movement parser
</commit_message>
<xml_diff>
--- a/bio_diversity/static/data_templates/measuring.xlsx
+++ b/bio_diversity/static/data_templates/measuring.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Individual" sheetId="3" r:id="rId1"/>
-    <sheet name="Group" sheetId="4" r:id="rId2"/>
+    <sheet name="Untagged" sheetId="4" r:id="rId2"/>
+    <sheet name="Group" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -307,8 +308,136 @@
 </comments>
 </file>
 
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+    <author>Stoyel, Quentin</author>
+  </authors>
+  <commentList>
+    <comment ref="A3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>eg. 1999</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>eg. Jan</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>eg. 1</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>eg. BSR</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>eg. Bonell</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F3" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Eg. 1999 BSR</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G3" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Fill in to record current container, or if movement occurred.  Leave blank if movement origin is unknown.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H3" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Fill in if a movement occurred, or if origin tank is unknown.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J3" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Did the group get split, or did it move as a whole?</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="24">
   <si>
     <t>PIT</t>
   </si>
@@ -374,6 +503,12 @@
   </si>
   <si>
     <t>ADDITIONAL COLUMNS</t>
+  </si>
+  <si>
+    <t>Number of Fish</t>
+  </si>
+  <si>
+    <t>Whole group (Y/N)</t>
   </si>
 </sst>
 </file>
@@ -507,7 +642,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -525,6 +660,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -844,19 +994,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="13"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="18"/>
     </row>
     <row r="3" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
@@ -1267,10 +1417,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:S71"/>
+  <dimension ref="A1:S71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1:N1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1287,22 +1437,23 @@
     <col min="19" max="19" width="14" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:19" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D2" s="2"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
-      <c r="J2" s="11" t="s">
+      <c r="J2" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="12"/>
-      <c r="P2" s="12"/>
-      <c r="Q2" s="12"/>
-      <c r="R2" s="12"/>
-      <c r="S2" s="13"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="17"/>
+      <c r="P2" s="17"/>
+      <c r="Q2" s="17"/>
+      <c r="R2" s="17"/>
+      <c r="S2" s="18"/>
     </row>
     <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
@@ -1649,4 +1800,71 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:K3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="5" width="9.140625" style="11"/>
+    <col min="6" max="6" width="13.5703125" style="11" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" style="11" customWidth="1"/>
+    <col min="8" max="8" width="16.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.42578125" style="11" customWidth="1"/>
+    <col min="10" max="10" width="18.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="11"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C2" s="12"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+    </row>
+    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="K3" s="15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add extra cols to grp parser
</commit_message>
<xml_diff>
--- a/bio_diversity/static/data_templates/measuring.xlsx
+++ b/bio_diversity/static/data_templates/measuring.xlsx
@@ -297,7 +297,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">UFID associated with a tissue sample, optional. 
 </t>
@@ -432,12 +432,38 @@
         </r>
       </text>
     </comment>
+    <comment ref="K3" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Optioanl, entry must match to Animal Detail Subjective Code in DB</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L3" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Optioanl, entry must match to Animal Detail Subjective Code in DB</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="26">
   <si>
     <t>PIT</t>
   </si>
@@ -509,6 +535,12 @@
   </si>
   <si>
     <t>Whole group (Y/N)</t>
+  </si>
+  <si>
+    <t>Vaccinated</t>
+  </si>
+  <si>
+    <t>Mark Applied</t>
   </si>
 </sst>
 </file>
@@ -518,7 +550,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -557,12 +589,6 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1804,10 +1830,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:K3"/>
+  <dimension ref="A2:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1818,16 +1844,17 @@
     <col min="8" max="8" width="16.42578125" style="11" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.42578125" style="11" customWidth="1"/>
     <col min="10" max="10" width="18.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="11"/>
+    <col min="11" max="12" width="18.140625" style="11" customWidth="1"/>
+    <col min="13" max="13" width="10.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="11"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C2" s="12"/>
       <c r="D2" s="13"/>
       <c r="E2" s="13"/>
     </row>
-    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
         <v>1</v>
       </c>
@@ -1858,7 +1885,13 @@
       <c r="J3" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="K3" s="15" t="s">
+      <c r="K3" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="L3" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="M3" s="15" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add mark and vaccinated to all generic parsers
</commit_message>
<xml_diff>
--- a/bio_diversity/static/data_templates/measuring.xlsx
+++ b/bio_diversity/static/data_templates/measuring.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Individual" sheetId="3" r:id="rId1"/>
@@ -123,7 +123,33 @@
         </r>
       </text>
     </comment>
+    <comment ref="O3" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Optioanl, entry must match to Animal Detail Subjective Code in DB</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="P3" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Optioanl, entry must match to Animal Detail Subjective Code in DB</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R3" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -304,6 +330,32 @@
         </r>
       </text>
     </comment>
+    <comment ref="S3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Optioanl, entry must match to Animal Detail Subjective Code in DB</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="T3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Optioanl, entry must match to Animal Detail Subjective Code in DB</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -463,7 +515,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="26">
   <si>
     <t>PIT</t>
   </si>
@@ -999,10 +1051,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:P71"/>
+  <dimension ref="A2:R71"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:L1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1013,13 +1065,17 @@
     <col min="6" max="6" width="19" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.28515625" customWidth="1"/>
     <col min="8" max="9" width="13" customWidth="1"/>
-    <col min="11" max="11" width="14.140625" customWidth="1"/>
-    <col min="13" max="13" width="14.140625" customWidth="1"/>
-    <col min="15" max="15" width="12" customWidth="1"/>
-    <col min="16" max="16" width="22" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.42578125" customWidth="1"/>
+    <col min="12" max="12" width="16.7109375" customWidth="1"/>
+    <col min="13" max="13" width="18.140625" customWidth="1"/>
+    <col min="14" max="14" width="17.5703125" customWidth="1"/>
+    <col min="15" max="15" width="12.5703125" customWidth="1"/>
+    <col min="16" max="16" width="16.5703125" customWidth="1"/>
+    <col min="17" max="17" width="12" customWidth="1"/>
+    <col min="18" max="18" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="E2" s="16" t="s">
         <v>19</v>
       </c>
@@ -1032,9 +1088,11 @@
       <c r="L2" s="17"/>
       <c r="M2" s="17"/>
       <c r="N2" s="17"/>
-      <c r="O2" s="18"/>
-    </row>
-    <row r="3" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O2" s="17"/>
+      <c r="P2" s="17"/>
+      <c r="Q2" s="18"/>
+    </row>
+    <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
@@ -1077,81 +1135,87 @@
       <c r="N3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="O3" s="9" t="s">
+      <c r="O3" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="P3" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q3" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="P3" s="10" t="s">
+      <c r="R3" s="10" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C4" s="2"/>
       <c r="D4" s="4"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C5" s="2"/>
       <c r="D5" s="4"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
     </row>
-    <row r="6" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C6" s="2"/>
       <c r="D6" s="4"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C7" s="2"/>
       <c r="D7" s="1"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C8" s="2"/>
       <c r="D8" s="1"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C9" s="2"/>
       <c r="D9" s="1"/>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C10" s="2"/>
       <c r="D10" s="1"/>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C11" s="2"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C12" s="2"/>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C13" s="2"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C14" s="2"/>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C15" s="2"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C16" s="2"/>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
@@ -1433,7 +1497,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="E2:O2"/>
+    <mergeCell ref="E2:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1443,10 +1507,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S71"/>
+  <dimension ref="A1:U71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="T9" sqref="T9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1459,12 +1523,12 @@
     <col min="14" max="14" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="20.140625" customWidth="1"/>
     <col min="17" max="17" width="16.28515625" customWidth="1"/>
-    <col min="18" max="18" width="22.140625" customWidth="1"/>
-    <col min="19" max="19" width="14" customWidth="1"/>
+    <col min="18" max="20" width="22.140625" customWidth="1"/>
+    <col min="21" max="21" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D2" s="2"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -1479,9 +1543,11 @@
       <c r="P2" s="17"/>
       <c r="Q2" s="17"/>
       <c r="R2" s="17"/>
-      <c r="S2" s="18"/>
-    </row>
-    <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S2" s="17"/>
+      <c r="T2" s="17"/>
+      <c r="U2" s="18"/>
+    </row>
+    <row r="3" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>17</v>
       </c>
@@ -1536,65 +1602,71 @@
       <c r="R3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="S3" s="9" t="s">
+      <c r="S3" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="T3" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="U3" s="9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D4" s="2"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D5" s="2"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
     </row>
@@ -1820,7 +1892,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="J2:S2"/>
+    <mergeCell ref="J2:U2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1832,8 +1904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
add status to generic indv parser
</commit_message>
<xml_diff>
--- a/bio_diversity/static/data_templates/measuring.xlsx
+++ b/bio_diversity/static/data_templates/measuring.xlsx
@@ -132,11 +132,25 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
+          <t xml:space="preserve">Release / Keep
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P3" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
           <t>Optioanl, entry must match to Animal Detail Subjective Code in DB</t>
         </r>
       </text>
     </comment>
-    <comment ref="P3" authorId="1" shapeId="0">
+    <comment ref="Q3" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -149,7 +163,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R3" authorId="1" shapeId="0">
+    <comment ref="S3" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -515,7 +529,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="27">
   <si>
     <t>PIT</t>
   </si>
@@ -593,6 +607,9 @@
   </si>
   <si>
     <t>Mark Applied</t>
+  </si>
+  <si>
+    <t>Status</t>
   </si>
 </sst>
 </file>
@@ -1051,10 +1068,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:R71"/>
+  <dimension ref="A2:S71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K34" sqref="K34"/>
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1068,14 +1085,14 @@
     <col min="11" max="11" width="21.42578125" customWidth="1"/>
     <col min="12" max="12" width="16.7109375" customWidth="1"/>
     <col min="13" max="13" width="18.140625" customWidth="1"/>
-    <col min="14" max="14" width="17.5703125" customWidth="1"/>
-    <col min="15" max="15" width="12.5703125" customWidth="1"/>
-    <col min="16" max="16" width="16.5703125" customWidth="1"/>
-    <col min="17" max="17" width="12" customWidth="1"/>
-    <col min="18" max="18" width="22" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="17.5703125" customWidth="1"/>
+    <col min="16" max="16" width="12.5703125" customWidth="1"/>
+    <col min="17" max="17" width="16.5703125" customWidth="1"/>
+    <col min="18" max="18" width="12" customWidth="1"/>
+    <col min="19" max="19" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="E2" s="16" t="s">
         <v>19</v>
       </c>
@@ -1090,9 +1107,10 @@
       <c r="N2" s="17"/>
       <c r="O2" s="17"/>
       <c r="P2" s="17"/>
-      <c r="Q2" s="18"/>
-    </row>
-    <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q2" s="17"/>
+      <c r="R2" s="18"/>
+    </row>
+    <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
@@ -1135,87 +1153,90 @@
       <c r="N3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="O3" s="14" t="s">
+      <c r="O3" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="P3" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="P3" s="14" t="s">
+      <c r="Q3" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="Q3" s="9" t="s">
+      <c r="R3" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="R3" s="10" t="s">
+      <c r="S3" s="10" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C4" s="2"/>
       <c r="D4" s="4"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C5" s="2"/>
       <c r="D5" s="4"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
     </row>
-    <row r="6" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C6" s="2"/>
       <c r="D6" s="4"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C7" s="2"/>
       <c r="D7" s="1"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C8" s="2"/>
       <c r="D8" s="1"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C9" s="2"/>
       <c r="D9" s="1"/>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C10" s="2"/>
       <c r="D10" s="1"/>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C11" s="2"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C12" s="2"/>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C13" s="2"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C14" s="2"/>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C15" s="2"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C16" s="2"/>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
@@ -1497,7 +1518,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="E2:Q2"/>
+    <mergeCell ref="E2:R2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update indv, group and sample detail list views
</commit_message>
<xml_diff>
--- a/bio_diversity/static/data_templates/measuring.xlsx
+++ b/bio_diversity/static/data_templates/measuring.xlsx
@@ -123,6 +123,19 @@
         </r>
       </text>
     </comment>
+    <comment ref="J3" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Vial Number, Optional</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="K3" authorId="1" shapeId="0">
       <text>
         <r>
@@ -134,6 +147,19 @@
           </rPr>
           <t>Use full name
 Eg. Fry/Parr/Smolt</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N3" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Scale Envelope number, optional</t>
         </r>
       </text>
     </comment>
@@ -359,6 +385,19 @@
         </r>
       </text>
     </comment>
+    <comment ref="N3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Vial Number, Optional</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="O3" authorId="0" shapeId="0">
       <text>
         <r>
@@ -382,8 +421,21 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">UFID associated with a tissue sample, optional. 
+          <t xml:space="preserve">UFID associated with a sample, optional. 
 </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="S3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Scale Envelope number, optional</t>
         </r>
       </text>
     </comment>
@@ -1149,7 +1201,7 @@
   <dimension ref="A2:T71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1613,8 +1665,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1624,6 +1676,7 @@
     <col min="10" max="10" width="23.140625" customWidth="1"/>
     <col min="12" max="12" width="13" customWidth="1"/>
     <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" customWidth="1"/>
     <col min="16" max="16" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="17" max="18" width="20.140625" customWidth="1"/>
     <col min="19" max="19" width="16.28515625" customWidth="1"/>

</xml_diff>